<commit_message>
Update test case ok
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DOCUNQUESRLXX/Docunque_SRL/Docunque/V.1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DOCUNQUESRLXX/Docunque_SRL/Docunque/V.1.0.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludo/GitHub/FSE2/PULL_REQUEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B07EC-B714-254C-9424-82438C75682E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC3B335-E5DB-9B49-AFF7-A51B1F9FFDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="29560" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4360" yWindow="760" windowWidth="30200" windowHeight="20200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4490,12 +4490,6 @@
     <t>Il caso di test fa riferimento ad un esempio CDA2 semplice in cui sono presenti solo le sezioni ed elementi obbligatori da specifiche nazionali HL7 Italia.</t>
   </si>
   <si>
-    <t>03c41b1574e25f32</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.7f401345c6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">3) Se il test è applicabile la colonna APPLICABILITA' deve essere compilata con SI e dovranno essere valorizzate:
     DATA ESECUZIONE, 
     TIMESTAMP, 
@@ -4510,30 +4504,6 @@
   </si>
   <si>
     <t>Il caso di test fa riferimento ad un esempio CDA2 in cui sono presenti le section obbligatorie e tutte le relative entry obbligatorie e opzionali, con alcuni sotto-elementi aggiuntivi le cui cardinalità sono riportate nel file excel.</t>
-  </si>
-  <si>
-    <t>95b931931416d4ba</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.a4de5c14f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6449cd11663ce48d</t>
-  </si>
-  <si>
-    <t>05250d5651da62ea</t>
-  </si>
-  <si>
-    <t>08d16bddc98332b8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.29712043cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.658d7e7c16^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.6ef94793de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Si prende in esame il caso di un assistito che è stato affetto da un ictus e che ha necessità di effettuare attività di riabilitazione sia motoria che di logopedia</t>
@@ -5430,6 +5400,36 @@
   </si>
   <si>
     <t>Il campo purpose_of_use non è corretto</t>
+  </si>
+  <si>
+    <t>c0a75b037e9dbce3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.bc485131e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>88d6e93a1045bb1c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.94aa7902bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>be1751d3e5efc8a5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.030927dab1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>6f36b4173d41641f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.aa3c172925^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4dafa1eaa1eeed39</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.f0949a9652^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -6255,7 +6255,7 @@
     </row>
     <row r="4" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8398,8 +8398,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N190" sqref="N190"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I382" sqref="I382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8444,7 +8444,7 @@
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="46" t="s">
-        <v>913</v>
+        <v>903</v>
       </c>
       <c r="D2" s="45"/>
       <c r="F2" s="11"/>
@@ -8469,7 +8469,7 @@
       </c>
       <c r="B3" s="48"/>
       <c r="C3" s="46" t="s">
-        <v>912</v>
+        <v>902</v>
       </c>
       <c r="D3" s="45"/>
       <c r="F3" s="11"/>
@@ -8492,7 +8492,7 @@
       <c r="A4" s="49"/>
       <c r="B4" s="50"/>
       <c r="C4" s="46" t="s">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="3"/>
@@ -8516,7 +8516,7 @@
       <c r="A5" s="51"/>
       <c r="B5" s="52"/>
       <c r="C5" s="46" t="s">
-        <v>911</v>
+        <v>901</v>
       </c>
       <c r="D5" s="45"/>
       <c r="F5" s="11"/>
@@ -9595,10 +9595,10 @@
         <v>45251.453587962962</v>
       </c>
       <c r="H37" s="23" t="s">
-        <v>916</v>
+        <v>906</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="J37" s="24" t="s">
         <v>137</v>
@@ -9611,13 +9611,13 @@
         <v>137</v>
       </c>
       <c r="N37" s="24" t="s">
-        <v>918</v>
+        <v>908</v>
       </c>
       <c r="O37" s="24" t="s">
         <v>826</v>
       </c>
       <c r="P37" s="24" t="s">
-        <v>919</v>
+        <v>909</v>
       </c>
       <c r="Q37" s="24"/>
       <c r="R37" s="25"/>
@@ -9887,10 +9887,10 @@
         <v>45251.46292824074</v>
       </c>
       <c r="H45" s="23" t="s">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="I45" s="23" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="J45" s="24" t="s">
         <v>137</v>
@@ -9903,13 +9903,13 @@
         <v>137</v>
       </c>
       <c r="N45" s="24" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="O45" s="24" t="s">
         <v>826</v>
       </c>
       <c r="P45" s="24" t="s">
-        <v>919</v>
+        <v>909</v>
       </c>
       <c r="Q45" s="24"/>
       <c r="R45" s="25"/>
@@ -10195,13 +10195,13 @@
         <v>137</v>
       </c>
       <c r="N53" s="24" t="s">
-        <v>914</v>
+        <v>904</v>
       </c>
       <c r="O53" s="24" t="s">
         <v>826</v>
       </c>
       <c r="P53" s="24" t="s">
-        <v>915</v>
+        <v>905</v>
       </c>
       <c r="Q53" s="24"/>
       <c r="R53" s="25" t="s">
@@ -14421,16 +14421,16 @@
         <v>827</v>
       </c>
       <c r="F177" s="22">
-        <v>45194</v>
+        <v>45257</v>
       </c>
       <c r="G177" s="36">
-        <v>45194.716122685182</v>
+        <v>45257.776446759257</v>
       </c>
       <c r="H177" s="23" t="s">
-        <v>828</v>
+        <v>914</v>
       </c>
       <c r="I177" s="23" t="s">
-        <v>829</v>
+        <v>915</v>
       </c>
       <c r="J177" s="24" t="s">
         <v>137</v>
@@ -14462,19 +14462,19 @@
         <v>381</v>
       </c>
       <c r="E178" s="33" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="F178" s="22">
-        <v>45194</v>
+        <v>45257</v>
       </c>
       <c r="G178" s="36">
-        <v>45194.720752314817</v>
+        <v>45257.763194444444</v>
       </c>
       <c r="H178" s="23" t="s">
-        <v>832</v>
+        <v>912</v>
       </c>
       <c r="I178" s="23" t="s">
-        <v>833</v>
+        <v>913</v>
       </c>
       <c r="J178" s="24" t="s">
         <v>137</v>
@@ -14506,19 +14506,19 @@
         <v>382</v>
       </c>
       <c r="E179" s="38" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="F179" s="22">
-        <v>45194</v>
+        <v>45257.780370370368</v>
       </c>
       <c r="G179" s="36">
-        <v>45194.724699074075</v>
+        <v>45257.780370370368</v>
       </c>
       <c r="H179" s="23" t="s">
-        <v>835</v>
+        <v>916</v>
       </c>
       <c r="I179" s="23" t="s">
-        <v>838</v>
+        <v>917</v>
       </c>
       <c r="J179" s="24" t="s">
         <v>137</v>
@@ -14550,19 +14550,19 @@
         <v>383</v>
       </c>
       <c r="E180" s="38" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
       <c r="F180" s="22">
-        <v>45194</v>
+        <v>45257.784456018519</v>
       </c>
       <c r="G180" s="36">
-        <v>45194.731261574074</v>
+        <v>45257.784456018519</v>
       </c>
       <c r="H180" s="23" t="s">
-        <v>836</v>
+        <v>918</v>
       </c>
       <c r="I180" s="23" t="s">
-        <v>837</v>
+        <v>919</v>
       </c>
       <c r="J180" s="24" t="s">
         <v>137</v>
@@ -14603,10 +14603,10 @@
         <v>45194.735902777778</v>
       </c>
       <c r="H181" s="23" t="s">
-        <v>846</v>
+        <v>836</v>
       </c>
       <c r="I181" s="23" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="J181" s="24" t="s">
         <v>137</v>
@@ -14619,13 +14619,13 @@
         <v>137</v>
       </c>
       <c r="N181" s="24" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="O181" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P181" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q181" s="24"/>
       <c r="R181" s="25"/>
@@ -14648,7 +14648,7 @@
         <v>387</v>
       </c>
       <c r="E182" s="38" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="F182" s="22">
         <v>45194</v>
@@ -14657,10 +14657,10 @@
         <v>45194.741400462961</v>
       </c>
       <c r="H182" s="23" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="I182" s="23" t="s">
-        <v>851</v>
+        <v>841</v>
       </c>
       <c r="J182" s="24" t="s">
         <v>137</v>
@@ -14673,13 +14673,13 @@
         <v>137</v>
       </c>
       <c r="N182" s="24" t="s">
-        <v>850</v>
+        <v>840</v>
       </c>
       <c r="O182" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P182" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q182" s="24"/>
       <c r="R182" s="25"/>
@@ -14702,7 +14702,7 @@
         <v>388</v>
       </c>
       <c r="E183" s="32" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="F183" s="22">
         <v>45194</v>
@@ -14711,10 +14711,10 @@
         <v>45194.748020833336</v>
       </c>
       <c r="H183" s="23" t="s">
-        <v>852</v>
+        <v>842</v>
       </c>
       <c r="I183" s="23" t="s">
-        <v>853</v>
+        <v>843</v>
       </c>
       <c r="J183" s="24" t="s">
         <v>137</v>
@@ -14727,13 +14727,13 @@
         <v>137</v>
       </c>
       <c r="N183" s="24" t="s">
-        <v>854</v>
+        <v>844</v>
       </c>
       <c r="O183" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P183" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q183" s="24"/>
       <c r="R183" s="25"/>
@@ -14756,7 +14756,7 @@
         <v>389</v>
       </c>
       <c r="E184" s="32" t="s">
-        <v>855</v>
+        <v>845</v>
       </c>
       <c r="F184" s="22">
         <v>45194</v>
@@ -14765,10 +14765,10 @@
         <v>45194.753391203703</v>
       </c>
       <c r="H184" s="23" t="s">
-        <v>868</v>
+        <v>858</v>
       </c>
       <c r="I184" s="23" t="s">
-        <v>869</v>
+        <v>859</v>
       </c>
       <c r="J184" s="24" t="s">
         <v>137</v>
@@ -14781,13 +14781,13 @@
         <v>137</v>
       </c>
       <c r="N184" s="24" t="s">
-        <v>870</v>
+        <v>860</v>
       </c>
       <c r="O184" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P184" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q184" s="24"/>
       <c r="R184" s="25"/>
@@ -14810,7 +14810,7 @@
         <v>390</v>
       </c>
       <c r="E185" s="38" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="F185" s="22">
         <v>45194</v>
@@ -14819,10 +14819,10 @@
         <v>45194.754710648151</v>
       </c>
       <c r="H185" s="23" t="s">
-        <v>873</v>
+        <v>863</v>
       </c>
       <c r="I185" s="23" t="s">
-        <v>874</v>
+        <v>864</v>
       </c>
       <c r="J185" s="24" t="s">
         <v>137</v>
@@ -14835,13 +14835,13 @@
         <v>137</v>
       </c>
       <c r="N185" s="24" t="s">
-        <v>871</v>
+        <v>861</v>
       </c>
       <c r="O185" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P185" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q185" s="24"/>
       <c r="R185" s="25"/>
@@ -14864,7 +14864,7 @@
         <v>391</v>
       </c>
       <c r="E186" s="32" t="s">
-        <v>857</v>
+        <v>847</v>
       </c>
       <c r="F186" s="22">
         <v>45194</v>
@@ -14873,10 +14873,10 @@
         <v>45194.757233796299</v>
       </c>
       <c r="H186" s="23" t="s">
-        <v>876</v>
+        <v>866</v>
       </c>
       <c r="I186" s="23" t="s">
-        <v>875</v>
+        <v>865</v>
       </c>
       <c r="J186" s="24" t="s">
         <v>137</v>
@@ -14889,13 +14889,13 @@
         <v>137</v>
       </c>
       <c r="N186" s="24" t="s">
-        <v>872</v>
+        <v>862</v>
       </c>
       <c r="O186" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P186" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q186" s="24"/>
       <c r="R186" s="25"/>
@@ -14918,7 +14918,7 @@
         <v>392</v>
       </c>
       <c r="E187" s="32" t="s">
-        <v>858</v>
+        <v>848</v>
       </c>
       <c r="F187" s="22">
         <v>45194</v>
@@ -14927,10 +14927,10 @@
         <v>45194.760578703703</v>
       </c>
       <c r="H187" s="23" t="s">
-        <v>877</v>
+        <v>867</v>
       </c>
       <c r="I187" s="23" t="s">
-        <v>878</v>
+        <v>868</v>
       </c>
       <c r="J187" s="24" t="s">
         <v>137</v>
@@ -14943,13 +14943,13 @@
         <v>137</v>
       </c>
       <c r="N187" s="24" t="s">
-        <v>879</v>
+        <v>869</v>
       </c>
       <c r="O187" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P187" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q187" s="24"/>
       <c r="R187" s="25"/>
@@ -14981,10 +14981,10 @@
         <v>45194.762465277781</v>
       </c>
       <c r="H188" s="23" t="s">
-        <v>880</v>
+        <v>870</v>
       </c>
       <c r="I188" s="23" t="s">
-        <v>881</v>
+        <v>871</v>
       </c>
       <c r="J188" s="24" t="s">
         <v>137</v>
@@ -14997,13 +14997,13 @@
         <v>137</v>
       </c>
       <c r="N188" s="24" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="O188" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P188" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q188" s="24"/>
       <c r="R188" s="25"/>
@@ -15026,7 +15026,7 @@
         <v>395</v>
       </c>
       <c r="E189" s="32" t="s">
-        <v>859</v>
+        <v>849</v>
       </c>
       <c r="F189" s="22">
         <v>45194</v>
@@ -15035,10 +15035,10 @@
         <v>45194.764699074076</v>
       </c>
       <c r="H189" s="23" t="s">
-        <v>883</v>
+        <v>873</v>
       </c>
       <c r="I189" s="23" t="s">
-        <v>884</v>
+        <v>874</v>
       </c>
       <c r="J189" s="24" t="s">
         <v>137</v>
@@ -15051,13 +15051,13 @@
         <v>137</v>
       </c>
       <c r="N189" s="24" t="s">
-        <v>885</v>
+        <v>875</v>
       </c>
       <c r="O189" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P189" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q189" s="24"/>
       <c r="R189" s="25"/>
@@ -15080,7 +15080,7 @@
         <v>396</v>
       </c>
       <c r="E190" s="32" t="s">
-        <v>860</v>
+        <v>850</v>
       </c>
       <c r="F190" s="22">
         <v>45251</v>
@@ -15089,10 +15089,10 @@
         <v>45251.429039351853</v>
       </c>
       <c r="H190" s="23" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="I190" s="23" t="s">
-        <v>909</v>
+        <v>899</v>
       </c>
       <c r="J190" s="24" t="s">
         <v>137</v>
@@ -15105,13 +15105,13 @@
         <v>137</v>
       </c>
       <c r="N190" s="24" t="s">
-        <v>907</v>
+        <v>897</v>
       </c>
       <c r="O190" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P190" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q190" s="24"/>
       <c r="R190" s="25"/>
@@ -15134,7 +15134,7 @@
         <v>397</v>
       </c>
       <c r="E191" s="32" t="s">
-        <v>861</v>
+        <v>851</v>
       </c>
       <c r="F191" s="22">
         <v>45194</v>
@@ -15143,10 +15143,10 @@
         <v>45194.773472222223</v>
       </c>
       <c r="H191" s="23" t="s">
-        <v>889</v>
+        <v>879</v>
       </c>
       <c r="I191" s="23" t="s">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="J191" s="24" t="s">
         <v>137</v>
@@ -15159,13 +15159,13 @@
         <v>137</v>
       </c>
       <c r="N191" s="24" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="O191" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P191" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q191" s="24"/>
       <c r="R191" s="25"/>
@@ -15188,7 +15188,7 @@
         <v>398</v>
       </c>
       <c r="E192" s="32" t="s">
-        <v>862</v>
+        <v>852</v>
       </c>
       <c r="F192" s="22">
         <v>45197</v>
@@ -15197,10 +15197,10 @@
         <v>45197.658148148148</v>
       </c>
       <c r="H192" s="23" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="I192" s="23" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
       <c r="J192" s="24" t="s">
         <v>137</v>
@@ -15213,13 +15213,13 @@
         <v>137</v>
       </c>
       <c r="N192" s="24" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="O192" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P192" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q192" s="24"/>
       <c r="R192" s="25"/>
@@ -15242,7 +15242,7 @@
         <v>399</v>
       </c>
       <c r="E193" s="32" t="s">
-        <v>863</v>
+        <v>853</v>
       </c>
       <c r="F193" s="22">
         <v>45197</v>
@@ -15251,10 +15251,10 @@
         <v>45197.660046296296</v>
       </c>
       <c r="H193" s="23" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="I193" s="23" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="J193" s="24" t="s">
         <v>137</v>
@@ -15267,13 +15267,13 @@
         <v>137</v>
       </c>
       <c r="N193" s="24" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="O193" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P193" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q193" s="24"/>
       <c r="R193" s="25"/>
@@ -15296,7 +15296,7 @@
         <v>400</v>
       </c>
       <c r="E194" s="38" t="s">
-        <v>864</v>
+        <v>854</v>
       </c>
       <c r="F194" s="22">
         <v>45197</v>
@@ -15305,10 +15305,10 @@
         <v>45197.655763888892</v>
       </c>
       <c r="H194" s="23" t="s">
-        <v>895</v>
+        <v>885</v>
       </c>
       <c r="I194" s="23" t="s">
-        <v>896</v>
+        <v>886</v>
       </c>
       <c r="J194" s="24" t="s">
         <v>137</v>
@@ -15321,13 +15321,13 @@
         <v>137</v>
       </c>
       <c r="N194" s="24" t="s">
-        <v>897</v>
+        <v>887</v>
       </c>
       <c r="O194" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P194" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q194" s="24"/>
       <c r="R194" s="25"/>
@@ -15350,7 +15350,7 @@
         <v>401</v>
       </c>
       <c r="E195" s="32" t="s">
-        <v>865</v>
+        <v>855</v>
       </c>
       <c r="F195" s="22">
         <v>45197</v>
@@ -15359,10 +15359,10 @@
         <v>45197.650925925926</v>
       </c>
       <c r="H195" s="23" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
       <c r="I195" s="23" t="s">
-        <v>893</v>
+        <v>883</v>
       </c>
       <c r="J195" s="24" t="s">
         <v>137</v>
@@ -15375,13 +15375,13 @@
         <v>137</v>
       </c>
       <c r="N195" s="24" t="s">
-        <v>894</v>
+        <v>884</v>
       </c>
       <c r="O195" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P195" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q195" s="24"/>
       <c r="R195" s="25"/>
@@ -15404,7 +15404,7 @@
         <v>402</v>
       </c>
       <c r="E196" s="41" t="s">
-        <v>866</v>
+        <v>856</v>
       </c>
       <c r="F196" s="22">
         <v>45243</v>
@@ -15413,10 +15413,10 @@
         <v>45243.677615740744</v>
       </c>
       <c r="H196" s="23" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="I196" s="23" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="J196" s="24" t="s">
         <v>137</v>
@@ -15429,13 +15429,13 @@
         <v>137</v>
       </c>
       <c r="N196" s="24" t="s">
-        <v>906</v>
+        <v>896</v>
       </c>
       <c r="O196" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P196" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q196" s="24"/>
       <c r="R196" s="25"/>
@@ -15458,7 +15458,7 @@
         <v>403</v>
       </c>
       <c r="E197" s="32" t="s">
-        <v>867</v>
+        <v>857</v>
       </c>
       <c r="F197" s="22">
         <v>45194</v>
@@ -15467,10 +15467,10 @@
         <v>45194.774178240739</v>
       </c>
       <c r="H197" s="23" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
       <c r="I197" s="23" t="s">
-        <v>887</v>
+        <v>877</v>
       </c>
       <c r="J197" s="24" t="s">
         <v>137</v>
@@ -15483,13 +15483,13 @@
         <v>137</v>
       </c>
       <c r="N197" s="24" t="s">
-        <v>888</v>
+        <v>878</v>
       </c>
       <c r="O197" s="24" t="s">
         <v>137</v>
       </c>
       <c r="P197" s="24" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="Q197" s="24"/>
       <c r="R197" s="25"/>
@@ -21768,19 +21768,19 @@
         <v>384</v>
       </c>
       <c r="E382" s="38" t="s">
-        <v>842</v>
+        <v>832</v>
       </c>
       <c r="F382" s="22">
-        <v>45194</v>
+        <v>45257.787245370368</v>
       </c>
       <c r="G382" s="36">
-        <v>45194.731388888889</v>
+        <v>45257.787245370368</v>
       </c>
       <c r="H382" s="23" t="s">
-        <v>834</v>
+        <v>920</v>
       </c>
       <c r="I382" s="23" t="s">
-        <v>839</v>
+        <v>921</v>
       </c>
       <c r="J382" s="24" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
Update test case 172
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DOCUNQUESRLXX/Docunque_SRL/Docunque/V.1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DOCUNQUESRLXX/Docunque_SRL/Docunque/V.1.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludo/GitHub/FSE2/PULL_REQUEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A32247-2A04-4F49-B1DB-977A83FE73DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863BF93F-5C1C-6F46-822D-B788A5C4682C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5420,16 +5420,16 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.03fe66fcee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>3347678a5dcd99b6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.7888746dca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>af6cd2afba9f3ad8</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.d366cc7c58^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>7da273b51e88366d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a9f4347f79cf3e1cf2ff4d79eaf6d0cf8d4a82cf3fb4e942adcc54e7fc27772e.5b77b1c491^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -8398,8 +8398,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E53" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I382" sqref="I382"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I180" sqref="I180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14553,16 +14553,16 @@
         <v>831</v>
       </c>
       <c r="F180" s="22">
-        <v>45260.529444444444</v>
+        <v>45264.510925925926</v>
       </c>
       <c r="G180" s="36">
-        <v>45260.535960648151</v>
+        <v>45264.510925925926</v>
       </c>
       <c r="H180" s="23" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="I180" s="23" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="J180" s="24" t="s">
         <v>137</v>
@@ -21777,10 +21777,10 @@
         <v>45260.537245370368</v>
       </c>
       <c r="H382" s="23" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="I382" s="23" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="J382" s="24" t="s">
         <v>137</v>

</xml_diff>